<commit_message>
Update thứ tự merging data
</commit_message>
<xml_diff>
--- a/Vietnam_Macro_Indicators_2010_2024.xlsx
+++ b/Vietnam_Macro_Indicators_2010_2024.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,16 @@
           <t>FDI Inflow (US$)</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Exports (% of GDP)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Imports (% of GDP)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -484,6 +494,12 @@
       <c r="F2" t="n">
         <v>8000000000</v>
       </c>
+      <c r="G2" t="n">
+        <v>54.1758459668515</v>
+      </c>
+      <c r="H2" t="n">
+        <v>59.8018415728627</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -504,6 +520,12 @@
       <c r="F3" t="n">
         <v>7430000000</v>
       </c>
+      <c r="G3" t="n">
+        <v>61.1801557211956</v>
+      </c>
+      <c r="H3" t="n">
+        <v>64.0804222196337</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -524,6 +546,12 @@
       <c r="F4" t="n">
         <v>8368000000</v>
       </c>
+      <c r="G4" t="n">
+        <v>63.4739249038633</v>
+      </c>
+      <c r="H4" t="n">
+        <v>59.7501918421214</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -544,6 +572,12 @@
       <c r="F5" t="n">
         <v>8900000000</v>
       </c>
+      <c r="G5" t="n">
+        <v>66.80044599191091</v>
+      </c>
+      <c r="H5" t="n">
+        <v>64.0459088748316</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -564,6 +598,12 @@
       <c r="F6" t="n">
         <v>9200000000</v>
       </c>
+      <c r="G6" t="n">
+        <v>69.5985759502054</v>
+      </c>
+      <c r="H6" t="n">
+        <v>65.8119455041556</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -584,6 +624,12 @@
       <c r="F7" t="n">
         <v>11800000000</v>
       </c>
+      <c r="G7" t="n">
+        <v>72.9228518369495</v>
+      </c>
+      <c r="H7" t="n">
+        <v>71.9913763582877</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -604,6 +650,12 @@
       <c r="F8" t="n">
         <v>12600000000</v>
       </c>
+      <c r="G8" t="n">
+        <v>74.10728625561831</v>
+      </c>
+      <c r="H8" t="n">
+        <v>71.3022217174998</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -624,6 +676,12 @@
       <c r="F9" t="n">
         <v>14100000000</v>
       </c>
+      <c r="G9" t="n">
+        <v>81.76252183556549</v>
+      </c>
+      <c r="H9" t="n">
+        <v>79.2175618233041</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -644,6 +702,12 @@
       <c r="F10" t="n">
         <v>15500000000</v>
       </c>
+      <c r="G10" t="n">
+        <v>84.4234560833365</v>
+      </c>
+      <c r="H10" t="n">
+        <v>80.2404806925565</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -664,6 +728,12 @@
       <c r="F11" t="n">
         <v>16120000000</v>
       </c>
+      <c r="G11" t="n">
+        <v>85.1575874073411</v>
+      </c>
+      <c r="H11" t="n">
+        <v>79.5466276240668</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -684,6 +754,12 @@
       <c r="F12" t="n">
         <v>15800000000</v>
       </c>
+      <c r="G12" t="n">
+        <v>84.381598008957</v>
+      </c>
+      <c r="H12" t="n">
+        <v>78.8642648059779</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -704,6 +780,12 @@
       <c r="F13" t="n">
         <v>15660000000</v>
       </c>
+      <c r="G13" t="n">
+        <v>93.8502071275575</v>
+      </c>
+      <c r="H13" t="n">
+        <v>92.8256257092568</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -724,6 +806,12 @@
       <c r="F14" t="n">
         <v>17900000000</v>
       </c>
+      <c r="G14" t="n">
+        <v>93.420129043511</v>
+      </c>
+      <c r="H14" t="n">
+        <v>89.7334901043249</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -744,6 +832,12 @@
       <c r="F15" t="n">
         <v>18500000000</v>
       </c>
+      <c r="G15" t="n">
+        <v>86.4674192371297</v>
+      </c>
+      <c r="H15" t="n">
+        <v>78.3506520327642</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -762,6 +856,8 @@
       <c r="F16" t="n">
         <v>20170000000</v>
       </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>